<commit_message>
added new file from Abhinav
</commit_message>
<xml_diff>
--- a/Lexbot.xlsx
+++ b/Lexbot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prabhsha/projects/aws-experiments/sumerian/lexbot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{742E9646-993D-F34E-96C6-001960D424C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD50C02C-FDC0-A94A-BE8F-D3595535CE5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="460" windowWidth="32580" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="125">
   <si>
     <t>CanSumerian</t>
   </si>
@@ -165,21 +165,12 @@
     <t>How is Sumerian different than Amazon Lumberyard?</t>
   </si>
   <si>
-    <t>Amazon Lumberyard and Amazon Sumerian are complimentary services that help customers design, build, and deploy 3D content. Sumerian and Lumberyard do share similarities in feature sets but serve different customer types. Sumerian uses technologies like JavaScript, HTML, WebGL, and WebVR to enable web and mobile developers to deploy experiences to target platforms through web browsers.</t>
-  </si>
-  <si>
     <t>How do I access Amazon Sumerian?</t>
   </si>
   <si>
-    <t>Amazon Sumerian is generally available. To get started access it from AWS console</t>
-  </si>
-  <si>
     <t>How much does Amazon Sumerian cost?</t>
   </si>
   <si>
-    <t>Please see our pricing page for the latest information.</t>
-  </si>
-  <si>
     <t>Does Sumerian integrate with other AWS services?</t>
   </si>
   <si>
@@ -309,26 +300,12 @@
     <t>augmented reality</t>
   </si>
   <si>
-    <t>Yes. We have integrated a base set of AWS services directly into the Sumerian interface, such as Amazon Polly for voice, or Amazon Cognito pool to fetch real-time data.
-To start integrating cloud services into your scenes, follow the IoT Thing Shadow and Script Actions tutorial.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon Lumberyard and Amazon Sumerian are complimentary services that help customers design, build, and deploy 3D content. Sumerian is designed to enable web and mobile developers to deploy experiences to target platforms through web browsers using technologies like JavaScript, HTML, WebGL, and WebVR to enable web and mobile developers </t>
-  </si>
-  <si>
     <t>ar</t>
   </si>
   <si>
     <t>slidetext</t>
   </si>
   <si>
-    <t>No specialized programming or 3D graphics expertise needed
-&lt;br&gt;
-Integrated development environment (IDE), editor, asset library, Hosts, and APIs for the design, development, and deployment of scenes
-&lt;br&gt;
-Get started with Amazon Sumerian for free. New customers can create up to a 50MB published scene equivalent to 100 views (5GB) per month, for 12 months</t>
-  </si>
-  <si>
     <t xml:space="preserve">Amazon Sumerian is a managed service that lets you create and run 3D, Augmented Reality and Virtual Reality applications. </t>
   </si>
   <si>
@@ -344,160 +321,206 @@
     <t>lumberyard</t>
   </si>
   <si>
-    <t>&lt;br&gt;
-For a list of supported browsers, please see the Amazon Sumerian Release Notes</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;
-For a list of supported platforms, please see the Amazon Sumerian Release Notes</t>
-  </si>
-  <si>
-    <t>&lt;br&gt; For latest information see &lt;a href="https://aws.amazon.com/releasenotes/?tag=releasenotes%23keywords%23amazon-sumerian"&gt;release notes&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>learn</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Sumerian supports the ARKit framework for augmented reality on iOS devices as well as ARCore for Android devices</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Turn text into lifelike speech to attract and hold audience attention
-&lt;br&gt;
-Dozens of lifelike voices across a variety of languages for apps to work in many different countries</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Understand and respond to the user’s speech
-&lt;br&gt;
-The Host/Avatar could respond with an answer or a question requesting more information about the inquiry
-&lt;br&gt;
-We have integrated a base set of AWS services directly into the Sumerian interface</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Multi-platform capability is a key feature in Sumerian
-&lt;br&gt;
-Sumerian currently supports Oculus Go, Oculus Rift, HTC Vive, HTC Vive Pro, Google Daydream, and Lenovo Mirage</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Polly lets you input text which your Host can speak in lifelike voices cross a variety of languages
-&lt;br&gt;
-Lex integration allows a conversational interface for your Host to understand and respond to users’ speech
-&lt;br&gt;
-To start integrating cloud services into your scenes, follow the IoT Thing Shadow and Script Actions tutorial</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Amazon Sumerian lets you create and run augmented reality (AR) applications without specialized expertise
-&lt;br&gt;
-Author your scene so that its objects are viewable in AR
-&lt;br&gt;
-The scripting system allows you to adjust the position of your objects as they appear in the real world</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;ul&gt;
-&lt;li&gt;Amazon Sumerian lets you create and run augmented reality (AR) applications without specialized expertise&lt;/li&gt;
-&lt;li&gt;Author your scene so that its objects are viewable in AR&lt;/li&gt;
-&lt;li&gt;The scripting system allows you to adjust the position of your objects as they appear in the real world&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Similarities in feature sets but serve different customer types
-&lt;img  width='500' src='https://i.imgur.com/qH184QN.png'&gt;</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Get started with Amazon Sumerian for free. New customers can create up to a 50MB published scene equivalent to 100 views (5GB) per month, for 12 months
-&lt;br&gt;
-For additional information and hands-on demos, join our 10 part twitch series on Developing VR/AR experiences at https://aws.amazon.com/developer/community/twitch/</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;Get started with Amazon Sumerian for free. New customers can create up to a 50MB published scene equivalent to 100 views (5GB) per month, for 12 months
-&lt;br&gt;
-No upfront costs or minimum fees
-&lt;br&gt;
-Pricing is based on:
-&lt;ol&gt;
-&lt;li&gt;Volume of Storage&lt;/li&gt;
-&lt;li&gt;Amount of Traffic&lt;/li&gt;
-&lt;li&gt;Other services used like Polly, Lex&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;No specialized programming or 3D graphics expertise needed
-&lt;br&gt;
-Integrated development environment (IDE), editor, asset library, Hosts, and APIs for the design, development, and deployment of scenes
-&lt;br&gt;
-Get started with Amazon Sumerian for free. New customers can create up to a 50MB published scene equivalent to 100 views (5GB) per month, for 12 months</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;All Amazon Sumerian customers have access to:
-&lt;ol&gt;
-&lt;li&gt;Documentation&lt;/li&gt;
-&lt;li&gt;Tutorials&lt;/li&gt;
-&lt;li&gt;Prebuilt scene templates and assets&lt;/li&gt;
-&lt;li&gt;Slack Channel&lt;/li&gt;
-&lt;li&gt;10 part series on Twitch&lt;/li&gt;
-&lt;/ol&gt;
-Additional support for via AWS Premium Support plans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;br&gt;You can build immersive and interactive scenes that run on AR and VR, mobile devices, and your web browser. </t>
-  </si>
-  <si>
-    <t>&lt;iframe width="500" height="200" src="https://www.youtube.com/embed/CMIXNu66fxs?autoplay=1" frameborder="0" allow="autoplay; encrypted-media" allowfullscreen&gt;&lt;/iframe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;
-&lt;h1&gt;WebVR&lt;/h1&gt;
-&lt;ul&gt;
-&lt;li&gt;Open specification to connect a VR headset to your computer and experience VR through your web browser&lt;/li&gt;
-&lt;li&gt;Popular headsets work better with certain browsers&lt;/li&gt;
-&lt;li&gt;For a list of supported browsers, please see the Amazon Sumerian Release Notes&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;&lt;br&gt;
-&lt;h2&gt;Technologies Sumerian is based on&lt;/h2&gt;
-&lt;ol&gt;
-&lt;li&gt;WebGL2&lt;/li&gt;
-&lt;li&gt;WebGL1 as fallback if WebGL2 is not available&lt;/li&gt;
-&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;br&gt;
-&lt;h1&gt;Amazon Sumerian&lt;/h1&gt;
-&lt;ul&gt;
-&lt;li&gt;Managed service - Create and run AR, VR and 3D apps&lt;/li&gt;
-&lt;li&gt;Multi-platform - Build immersive and interactive scenes that run on AR and VR, mobile devices, and web browser&lt;/li&gt;
-&lt;li&gt;Extensibility - Quickly add connections in your scenes to existing AWS services&lt;/li&gt;
-&lt;ul&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;br&gt;
-&lt;h1&gt;WebGL&lt;/h1&gt;
-&lt;ul&gt;
-    &lt;li&gt;JavaScript API used for rendering interactive 2D and 3D graphics in a browser&lt;/li&gt;
-    &lt;li&gt;WebGL is integrated completely into all the web standards of the browser, allowing GPU-accelerated usage of physics and image processing and effects as part of the web page canvas&lt;/li&gt;
-&lt;/ul&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-&lt;h1&gt;Amazon Sumerian&lt;/h1&gt;
-&lt;ul&gt;
-&lt;li&gt;Managed service - Create and run AR, VR and 3D apps&lt;/li&gt;
-&lt;li&gt;Multi-platform - Build immersive and interactive scenes that run on AR and VR, mobile devices, and web browser&lt;/li&gt;
-&lt;li&gt;Extensibility - Quickly add connections in your scenes to existing AWS services&lt;/li&gt;
-&lt;ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;h2&gt;File type support&lt;/h2&gt;
-Supports file types FBX 2017 and OBJ
-&lt;br&gt;
-Based on WebGL 2. Sumerian falls back to WebGL 1 where WebGL 2 is not available
-&lt;br&gt;
-For a list of supported browsers, please see the Amazon Sumerian Release Notes</t>
   </si>
   <si>
     <t xml:space="preserve">
 &lt;img  height="250" src="https://d1.awsstatic.com/Developer%20Marketing/DevOps/Amazon%20Sumerian/SumerianGA.3447d10e856380de77e9a9f3114db0f545c24b66.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe style ="position: absolute;top:0;left:0;width:100%;height:100%" src="https://www.youtube.com/embed/CMIXNu66fxs?autoplay=1" frameborder="0" allow="autoplay; encrypted-media" allowfullscreen&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:left; display: table"&gt;
+&lt;ul style="color:white; vertical-align: middle; display: table-cell"&gt;
+&lt;lh&gt;&lt;h1&gt;WebVR&lt;/h1&gt;&lt;/lh&gt;
+&lt;li&gt;Open specification to connect a VR headset to your computer and experience VR through your web browser&lt;/li&gt;
+&lt;br&gt;&lt;li&gt;Popular headsets work better with certain browsers&lt;/li&gt;
+&lt;br&gt;&lt;li&gt;For a list of supported browsers, please see the Amazon Sumerian Release Notes&lt;/li&gt;
+&lt;ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:left; display: table"&gt;
+&lt;ul style="color:white; vertical-align: middle; display: table-cell"&gt;
+&lt;lh&gt;&lt;h2&gt;File Type Support&lt;/h2&gt;&lt;/lh&gt;
+&lt;lh&gt;Supports file types FBX 2017 and OBJ&lt;/lh&gt;
+&lt;br&gt;
+&lt;br&gt;
+&lt;lh&gt;Based on WebGL 2. Sumerian falls back to WebGL 1 where WebGL 2 is not available&lt;/lh&gt;
+&lt;br&gt;
+&lt;br&gt;
+&lt;lh&gt;For a list of supported browsers, please see the Amazon Sumerian Release Notes&lt;/lh&gt;
+&lt;ul&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+For latest information see &lt;a href="https://aws.amazon.com/releasenotes/?tag=releasenotes%23keywords%23amazon-sumerian"&gt;release notes&lt;/a&gt;
+&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:left; display: table"&gt;
+&lt;ol style="color:white; vertical-align: middle; display: table-cell"&gt;
+&lt;lh&gt;All Amazon Sumerian customers have access to:&lt;/lh&gt;
+&lt;br&gt;
+&lt;br&gt;
+&lt;li&gt;Documentation&lt;/li&gt;
+&lt;br&gt;
+&lt;br&gt;
+&lt;li&gt;Tutorials&lt;/li&gt;
+&lt;br&gt;
+&lt;br&gt;
+&lt;li&gt;Prebuilt scene templates and assets&lt;/li&gt;
+&lt;br&gt;
+&lt;br&gt;
+&lt;li&gt;Slack Channel&lt;/li&gt;
+&lt;br&gt;
+&lt;br&gt;
+&lt;li&gt;10 part series on Twitch&lt;/li&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+You can build immersive and interactive scenes that run on AR and VR, mobile devices, and your web browser.&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+For a list of supported platforms, please see the Amazon Sumerian Release Notes
+&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+For a list of supported browsers, please see the Amazon Sumerian Release Notes
+&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img height="120" width="120" src="https://i.imgur.com/nrMn1vb.png"&gt;
+&lt;img height="120" width="120" src="https://i.imgur.com/290VwjM.png"&gt;
+&lt;img height="120" width="120" src="https://i.imgur.com/wYm3sny.jpg"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+Amazon Polly&lt;br&gt;Turn text into lifelike Speech&lt;br&gt;53 voices in 27 Languages&lt;br&gt;Available in 16 AWS regions&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+Common Use Cases
+&lt;br&gt;
+Employee Education
+&lt;br&gt;Field Service Productivity
+&lt;br&gt;Training Simulations
+&lt;br&gt;Virtual Concierge
+&lt;br&gt;Design &amp; Creative
+&lt;br&gt;Retail &amp; Sales&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img height="120" width="120" src="https://i.imgur.com/rHF6GQM.png"&gt;
+&lt;img height="120" width="120" src="https://i.imgur.com/VQnqGtv.jpg"&gt;
+&lt;img height="120" width="120" src="https://i.imgur.com/AH83rnz.png"&gt;
+&lt;br&gt;
+&lt;img height="120" width="120" src="https://i.imgur.com/eV8MY7U.png"&gt;
+&lt;img height="120" width="120" src="https://i.imgur.com/gqhrZA9.png"&gt;
+&lt;img height="120" width="120" src="https://i.imgur.com/qOlWXu4.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="height:100%;width:100%;text-align:center;"&gt;
+&lt;p style="vertical-align: middle"&gt;
+Amazon Polly
+&lt;br&gt;
+Amazon Lex
+&lt;br&gt;
+Amazon Cognito
+&lt;br&gt;
+To Get Started
+&lt;br&gt;
+&lt;img width="500" src="https://i.imgur.com/uzcDqyK.png"&gt;
+&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img width="450" src="https://i.imgur.com/m6wyUJB.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:left; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+Sumerian - The fastest and easiest way to create VR, AR, and 3D experiences
+&lt;br&gt;
+&lt;br&gt;Lumberyard - Build your most ambitious games
+&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+New to Sumerian?&lt;br&gt;Try AWS Sumerian for free in your first year of using the service&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+No upfront costs or minimum fees&lt;br&gt;Priced by storage and traffic&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Great news! You can get started with Sumerian for free. And as always, check our pricing page which has the latest information.</t>
+  </si>
+  <si>
+    <t>You can access Amazon Sumerian from the AWS console</t>
+  </si>
+  <si>
+    <t>They are complementary services that help customers design, build, and deploy 3D content. Sumerian and Lumberyard do share similarities in feature sets but serve different customer types</t>
+  </si>
+  <si>
+    <t>Yes. We have integrated a base set of AWS services directly into the Sumerian interface, such as Amazon Polly for voice, or Amazon Cognito pool to fetch real-time data.</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:center; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+Get started with Amazon Sumerian for free&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;img width="500" src="https://i.imgur.com/XA3RaIe.png"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:left; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+NO VR/AR EXPERTISE NEEDED
+&lt;br&gt;
+LIFELIKE CHARACTERS
+&lt;br&gt;
+DESIGN IMMERSIVE ENVIRONMENTS
+&lt;br&gt;
+RUN ON MULTIPLE PLATFORMS
+&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:left; display: table"&gt;
+&lt;p style="color:white; vertical-align: middle; display: table-cell"&gt;
+JavaScript API used for rendering interactive 2D and 3D graphics in a browser
+&lt;br&gt;
+Allow GPU-accelerated usage of physics and image processing and effects as part of the web page canvas
+&lt;/p&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div style="background-color:black;height:100%;width:100%;text-align:left; display: table"&gt;
+&lt;img src="https://i.imgur.com/qnbc9XO.png"&gt;
+&lt;/div&gt;</t>
   </si>
 </sst>
 </file>
@@ -865,8 +888,8 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -881,7 +904,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>37</v>
@@ -899,10 +922,10 @@
         <v>41</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -925,7 +948,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -948,7 +971,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -971,7 +994,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -994,7 +1017,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1005,19 +1028,19 @@
         <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1028,180 +1051,180 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>82</v>
       </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>85</v>
-      </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="112" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1215,16 +1238,16 @@
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="192" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1238,16 +1261,16 @@
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1270,7 +1293,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1293,7 +1316,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1310,13 +1333,13 @@
         <v>44</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1327,19 +1350,19 @@
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1350,88 +1373,88 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
         <v>70</v>
       </c>
-      <c r="D24" t="s">
-        <v>73</v>
-      </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1448,13 +1471,13 @@
         <v>23</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1465,7 +1488,7 @@
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
         <v>24</v>
@@ -1474,10 +1497,10 @@
         <v>25</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="176" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1488,7 +1511,7 @@
         <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
@@ -1497,10 +1520,10 @@
         <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1517,13 +1540,13 @@
         <v>23</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1540,13 +1563,13 @@
         <v>26</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1563,13 +1586,13 @@
         <v>23</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1580,7 +1603,7 @@
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
         <v>28</v>
@@ -1589,10 +1612,10 @@
         <v>27</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1603,7 +1626,7 @@
         <v>19</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
         <v>28</v>
@@ -1612,10 +1635,10 @@
         <v>27</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="144" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1626,7 +1649,7 @@
         <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
         <v>28</v>
@@ -1635,10 +1658,10 @@
         <v>27</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="255" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1658,10 +1681,10 @@
         <v>30</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="96" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1681,10 +1704,10 @@
         <v>33</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1704,10 +1727,10 @@
         <v>35</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1724,13 +1747,13 @@
         <v>26</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="160" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="340" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1750,10 +1773,10 @@
         <v>43</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1764,42 +1787,42 @@
         <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
         <v>19</v>
       </c>
       <c r="D40" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E40" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G40" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1810,7 +1833,7 @@
         <v>19</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E41" t="s">
         <v>34</v>
@@ -1819,53 +1842,53 @@
         <v>35</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="128" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D43" t="s">
         <v>17</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>